<commit_message>
Adding front page search with codes to test case 627
</commit_message>
<xml_diff>
--- a/test_files/filter_1_Code_list_three_extensions.xlsx
+++ b/test_files/filter_1_Code_list_three_extensions.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21723"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21803"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FD93B210-CE11-450B-9219-4CC982B6D42C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B34A30D1-9630-4AEC-AAA2-8493570C1DB7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" firstSheet="4" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CodeSchemes" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="185">
   <si>
     <t>CODEVALUE</t>
   </si>
@@ -346,6 +346,9 @@
   </si>
   <si>
     <t>Test code 25</t>
+  </si>
+  <si>
+    <t>RTT555</t>
   </si>
   <si>
     <t>PROPERTYTYPE</t>
@@ -974,7 +977,7 @@
   </sheetPr>
   <dimension ref="A1:P1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -2093,7 +2096,9 @@
   </sheetPr>
   <dimension ref="A1:J1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0" xr3:uid="{958C4451-9541-5A59-BF78-D2F731DF1C81}"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -2834,7 +2839,20 @@
         <v>43855</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="15.75" customHeight="1"/>
+    <row r="27" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A27" t="s">
+        <v>106</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I27" s="3">
+        <v>43126</v>
+      </c>
+      <c r="J27" s="3">
+        <v>43856</v>
+      </c>
+    </row>
     <row r="28" spans="1:10" ht="15.75" customHeight="1"/>
     <row r="29" spans="1:10" ht="15.75" customHeight="1"/>
     <row r="30" spans="1:10" ht="15.75" customHeight="1"/>
@@ -3820,7 +3838,7 @@
   </sheetPr>
   <dimension ref="A1:I1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0" xr3:uid="{842E5F09-E766-5B8D-85AF-A39847EA96FD}"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -3841,10 +3859,10 @@
         <v>3</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>8</v>
@@ -3859,18 +3877,18 @@
         <v>11</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="15.75" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="1"/>
@@ -3882,18 +3900,18 @@
         <v>24</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="15.75" customHeight="1">
       <c r="A3" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="1"/>
@@ -3905,27 +3923,27 @@
         <v>24</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="15.75" customHeight="1">
       <c r="A4" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G4" s="4">
         <v>42735</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="15.75" customHeight="1"/>
@@ -4936,7 +4954,7 @@
   </sheetPr>
   <dimension ref="A1:G1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0" xr3:uid="{51F8DEE0-4D01-5F28-A812-FC0BD7CAC4A5}">
+    <sheetView workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
@@ -4948,7 +4966,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" customHeight="1">
       <c r="A1" s="4" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>8</v>
@@ -4957,7 +4975,7 @@
         <v>9</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>30</v>
@@ -4974,10 +4992,10 @@
         <v>31</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>19</v>
@@ -4995,13 +5013,13 @@
         <v>35</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="E3" s="5"/>
       <c r="F3" s="3">
@@ -5016,13 +5034,13 @@
         <v>38</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>126</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>125</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="3">
@@ -5037,10 +5055,10 @@
         <v>41</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="5"/>
@@ -5056,13 +5074,13 @@
         <v>44</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="E6" s="5"/>
       <c r="F6" s="3">
@@ -5077,13 +5095,13 @@
         <v>20</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="E7" s="5"/>
       <c r="F7" s="3">
@@ -5098,10 +5116,10 @@
         <v>49</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="5"/>
@@ -5117,10 +5135,10 @@
         <v>52</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="5"/>
@@ -5136,10 +5154,10 @@
         <v>55</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="5"/>
@@ -6152,7 +6170,7 @@
   </sheetPr>
   <dimension ref="A1:I1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" xr3:uid="{F9CF3CF3-643B-5BE6-8B46-32C596A47465}">
+    <sheetView workbookViewId="0">
       <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
@@ -6163,13 +6181,13 @@
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>8</v>
@@ -6178,7 +6196,7 @@
         <v>9</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>30</v>
@@ -6192,19 +6210,19 @@
     </row>
     <row r="2" spans="1:9" ht="15.75" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>52</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>19</v>
@@ -6219,22 +6237,22 @@
     </row>
     <row r="3" spans="1:9" ht="15.75" customHeight="1">
       <c r="A3" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>55</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="G3" s="5"/>
       <c r="H3" s="3">
@@ -6246,22 +6264,22 @@
     </row>
     <row r="4" spans="1:9" ht="15.75" customHeight="1">
       <c r="A4" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>58</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="G4" s="5"/>
       <c r="H4" s="3">
@@ -6273,19 +6291,19 @@
     </row>
     <row r="5" spans="1:9" ht="15.75" customHeight="1">
       <c r="A5" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>61</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="5"/>
@@ -6298,19 +6316,19 @@
     </row>
     <row r="6" spans="1:9" ht="15.75" customHeight="1">
       <c r="A6" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>64</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="5"/>
@@ -6323,22 +6341,22 @@
     </row>
     <row r="7" spans="1:9" ht="15.75" customHeight="1">
       <c r="A7" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>67</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="G7" s="5"/>
       <c r="H7" s="3">
@@ -6350,22 +6368,22 @@
     </row>
     <row r="8" spans="1:9" ht="15.75" customHeight="1">
       <c r="A8" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>70</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="G8" s="5"/>
       <c r="H8" s="3">
@@ -6377,22 +6395,22 @@
     </row>
     <row r="9" spans="1:9" ht="15.75" customHeight="1">
       <c r="A9" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>73</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="G9" s="5"/>
       <c r="H9" s="3">
@@ -6404,19 +6422,19 @@
     </row>
     <row r="10" spans="1:9" ht="15.75" customHeight="1">
       <c r="A10" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>76</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="5"/>
@@ -7429,7 +7447,7 @@
   </sheetPr>
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView workbookViewId="0" xr3:uid="{78B4E459-6924-5F8B-B7BA-2DD04133E49E}"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -7441,7 +7459,7 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="4" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>8</v>
@@ -7450,7 +7468,7 @@
         <v>9</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>30</v>
@@ -7467,10 +7485,10 @@
         <v>31</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>19</v>
@@ -7488,13 +7506,13 @@
         <v>35</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="E3" s="5"/>
       <c r="F3" s="3">
@@ -7509,10 +7527,10 @@
         <v>38</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D4" s="7"/>
       <c r="E4" s="5"/>
@@ -7528,13 +7546,13 @@
         <v>41</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="E5" s="5"/>
       <c r="F5" s="3">
@@ -7549,10 +7567,10 @@
         <v>44</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="5"/>
@@ -7568,10 +7586,10 @@
         <v>20</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="5"/>
@@ -7587,10 +7605,10 @@
         <v>49</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="5"/>
@@ -7606,10 +7624,10 @@
         <v>52</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="5"/>
@@ -7625,10 +7643,10 @@
         <v>55</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="5"/>
@@ -7644,10 +7662,10 @@
         <v>58</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="F11" s="3">
         <v>43110</v>
@@ -7661,10 +7679,10 @@
         <v>61</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="F12" s="3">
         <v>43111</v>
@@ -7678,10 +7696,10 @@
         <v>64</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="F13" s="3">
         <v>43112</v>
@@ -7695,10 +7713,10 @@
         <v>67</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F14" s="3">
         <v>43113</v>
@@ -7712,10 +7730,10 @@
         <v>70</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="F15" s="3">
         <v>43114</v>
@@ -7729,10 +7747,10 @@
         <v>73</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="F16" s="3">
         <v>43115</v>
@@ -7746,10 +7764,10 @@
         <v>76</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F17" s="3">
         <v>43116</v>
@@ -7763,10 +7781,10 @@
         <v>79</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="F18" s="3">
         <v>43117</v>
@@ -7780,10 +7798,10 @@
         <v>82</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="F19" s="3">
         <v>43118</v>
@@ -7797,10 +7815,10 @@
         <v>85</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="F20" s="3">
         <v>43119</v>
@@ -7814,10 +7832,10 @@
         <v>88</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="F21" s="3">
         <v>43120</v>
@@ -7831,10 +7849,10 @@
         <v>91</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="F22" s="3">
         <v>43121</v>
@@ -7848,10 +7866,10 @@
         <v>94</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="F23" s="3">
         <v>43122</v>
@@ -7865,10 +7883,10 @@
         <v>97</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="F24" s="3">
         <v>43123</v>
@@ -7882,10 +7900,10 @@
         <v>100</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="F25" s="3">
         <v>43124</v>
@@ -7899,10 +7917,10 @@
         <v>103</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="F26" s="3">
         <v>43125</v>

</xml_diff>